<commit_message>
print accuracy in webpage complated
</commit_message>
<xml_diff>
--- a/multiRF.xlsx
+++ b/multiRF.xlsx
@@ -447,20 +447,20 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bwd iat max</t>
+          <t xml:space="preserve"> fwd header length</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.07138595656320885</v>
+        <v>0.05352177463688457</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -468,46 +468,46 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.06580167155027998</v>
+        <v>0.05132114164522052</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>bwd iat total</t>
+          <t xml:space="preserve"> idle max</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.05929263023110939</v>
+        <v>0.05079032304311388</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bwd iat std</t>
+          <t>fwd packets/s</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.05721439666707018</v>
+        <v>0.04765685279244385</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> idle max</t>
+          <t xml:space="preserve"> bwd iat mean</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.04530022156900686</v>
+        <v>0.04715369417577813</v>
       </c>
     </row>
     <row r="7">
@@ -516,115 +516,115 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bwd iat mean</t>
+          <t>bwd iat total</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.04498480878834067</v>
+        <v>0.04525872297014155</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total fwd packets</t>
+          <t>idle mean</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.04090381374051117</v>
+        <v>0.0398545026066294</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd header length</t>
+          <t xml:space="preserve"> bwd iat std</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.03385639837261451</v>
+        <v>0.03650224955751528</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bwd packets/s</t>
+          <t xml:space="preserve"> fwd iat min</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.03177957861611506</v>
+        <v>0.03148568619238207</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>unnamed: 0</t>
+          <t xml:space="preserve"> bwd iat min</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.02472154790009787</v>
+        <v>0.02858958990602306</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> destination port</t>
+          <t xml:space="preserve"> flow duration</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.02407050255922675</v>
+        <v>0.02721170215440187</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> source port</t>
+          <t>unnamed: 0</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.02370090951395776</v>
+        <v>0.02497444816996061</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>idle mean</t>
+          <t xml:space="preserve"> source port</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.02325869152699471</v>
+        <v>0.02344772370138886</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>fwd packets/s</t>
+          <t xml:space="preserve"> destination port</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.02202035405046929</v>
+        <v>0.02326241074107733</v>
       </c>
     </row>
     <row r="16">
@@ -633,128 +633,128 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total backward packets</t>
+          <t xml:space="preserve"> total fwd packets</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.0118270531963731</v>
+        <v>0.01619763551876954</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> idle std</t>
+          <t xml:space="preserve"> bwd iat max</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.01034325352639817</v>
+        <v>0.00868639303857755</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> subflow bwd packets</t>
+          <t xml:space="preserve"> init_win_bytes_backward</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.007684661234878386</v>
+        <v>0.007685638186746611</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> init_win_bytes_backward</t>
+          <t xml:space="preserve"> fwd header length.1</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.00758339524528518</v>
+        <v>0.007272873338239656</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> min_seg_size_forward</t>
+          <t>init_win_bytes_forward</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.007417852564032557</v>
+        <v>0.007086391199984689</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd header length.1</t>
+          <t>subflow fwd packets</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.007221518914639419</v>
+        <v>0.006994157484101189</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd packet length max</t>
+          <t xml:space="preserve"> bwd packets/s</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.007143854309332002</v>
+        <v>0.006187803114247391</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>subflow fwd packets</t>
+          <t xml:space="preserve"> total backward packets</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.006583511672593014</v>
+        <v>0.00578090648389456</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bwd iat min</t>
+          <t xml:space="preserve"> subflow bwd packets</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.005784283803613971</v>
+        <v>0.005058150279394818</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>init_win_bytes_forward</t>
+          <t xml:space="preserve"> idle std</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.004508464876965565</v>
+        <v>0.004314152961778288</v>
       </c>
     </row>
     <row r="26">
@@ -763,59 +763,59 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> flow duration</t>
+          <t xml:space="preserve"> protocol</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.0002555216491016057</v>
+        <v>0.003260901756261592</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> active max</t>
+          <t xml:space="preserve"> fwd packet length max</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>0.003239827766553275</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> active min</t>
+          <t xml:space="preserve"> flow packets/s</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>0.001769433015466189</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> active std</t>
+          <t xml:space="preserve"> flow iat mean</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>0.001540208623576104</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> flow iat max</t>
+          <t xml:space="preserve"> active max</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -824,11 +824,11 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> flow iat mean</t>
+          <t xml:space="preserve"> active min</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -837,11 +837,11 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> flow iat min</t>
+          <t xml:space="preserve"> active std</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -850,11 +850,11 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> flow iat std</t>
+          <t xml:space="preserve"> bwd packet length mean</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -863,11 +863,11 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> flow packets/s</t>
+          <t xml:space="preserve"> flow iat max</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -876,11 +876,11 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd iat max</t>
+          <t xml:space="preserve"> flow iat min</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -889,11 +889,11 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd iat mean</t>
+          <t xml:space="preserve"> flow iat std</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd iat min</t>
+          <t xml:space="preserve"> fwd iat max</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd iat std</t>
+          <t xml:space="preserve"> fwd iat mean</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -928,11 +928,11 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>active mean</t>
+          <t xml:space="preserve"> fwd iat std</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -941,11 +941,11 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>flow bytes/s</t>
+          <t>active mean</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -954,7 +954,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
add gif background in output display
</commit_message>
<xml_diff>
--- a/multiRF.xlsx
+++ b/multiRF.xlsx
@@ -447,7 +447,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -455,38 +455,38 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.07120417058558604</v>
+        <v>0.07009444328808008</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bwd iat mean</t>
+          <t xml:space="preserve"> idle max</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.06703151232954908</v>
+        <v>0.05567748014892089</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>bwd iat total</t>
+          <t xml:space="preserve"> bwd iat max</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.05995108186948368</v>
+        <v>0.05497377445208571</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -494,25 +494,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0585112840617725</v>
+        <v>0.0431655213575495</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> idle max</t>
+          <t>fwd packets/s</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.05718907297094</v>
+        <v>0.03994946027734891</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -520,59 +520,59 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0541521270126408</v>
+        <v>0.03931393056833637</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bwd iat max</t>
+          <t xml:space="preserve"> total fwd packets</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.04630576553115971</v>
+        <v>0.03749143573496819</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>fwd packets/s</t>
+          <t xml:space="preserve"> bwd iat min</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.04402592989656402</v>
+        <v>0.03593683107961872</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd header length</t>
+          <t xml:space="preserve"> ack flag count</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.03598119176475211</v>
+        <v>0.03349862431720758</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> flow duration</t>
+          <t xml:space="preserve"> bwd iat mean</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.03289109292571116</v>
+        <v>0.03204020489641801</v>
       </c>
     </row>
     <row r="12">
@@ -585,150 +585,150 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.02454376556058581</v>
+        <v>0.0251850571907887</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> source port</t>
+          <t xml:space="preserve"> destination port</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.02442606149750248</v>
+        <v>0.02452036515724147</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> destination port</t>
+          <t xml:space="preserve"> source port</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.0242472253583645</v>
+        <v>0.02435819388376988</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total fwd packets</t>
+          <t>idle mean</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.0191779146897114</v>
+        <v>0.01896168417342714</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>idle mean</t>
+          <t xml:space="preserve"> total backward packets</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.01755992285557451</v>
+        <v>0.012520814218368</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> subflow bwd packets</t>
+          <t xml:space="preserve"> fwd header length</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.007989803673089654</v>
+        <v>0.009896735672572786</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>subflow fwd packets</t>
+          <t xml:space="preserve"> init_win_bytes_backward</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.007740463428100431</v>
+        <v>0.00852979916262573</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> init_win_bytes_backward</t>
+          <t xml:space="preserve"> bwd packet length std</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.007589979381102729</v>
+        <v>0.00792086920103245</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total backward packets</t>
+          <t>subflow fwd packets</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.006202371172609173</v>
+        <v>0.007387838174065207</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bwd iat min</t>
+          <t xml:space="preserve"> subflow bwd packets</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.006079844724911699</v>
+        <v>0.006768837678581953</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fwd header length.1</t>
+          <t xml:space="preserve"> min_seg_size_forward</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.005820697367098386</v>
+        <v>0.006669714143792963</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> min_seg_size_forward</t>
+          <t xml:space="preserve"> fwd header length.1</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.005784590038017543</v>
+        <v>0.005859818094367625</v>
       </c>
     </row>
     <row r="24">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.005731714562681709</v>
+        <v>0.00445452626497436</v>
       </c>
     </row>
     <row r="25">
@@ -754,33 +754,33 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.004441472619692514</v>
+        <v>0.004388076194057555</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> protocol</t>
+          <t>fwd iat total</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.001820584329384103</v>
+        <v>0.001476827295665777</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>total length of fwd packets</t>
+          <t xml:space="preserve"> flow duration</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.001456867931392835</v>
+        <v>0.0001137145064307649</v>
       </c>
     </row>
     <row r="28">
@@ -824,7 +824,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -850,7 +850,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -863,7 +863,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -876,7 +876,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -889,7 +889,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -902,7 +902,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -915,7 +915,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -954,11 +954,11 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>fwd iat total</t>
+          <t>bwd iat total</t>
         </is>
       </c>
       <c r="C41" t="n">

</xml_diff>